<commit_message>
updated test cases and test plan
</commit_message>
<xml_diff>
--- a/Self_Learning_Testcases_and_results/Capstone_Self_Learning_Test_Cases_Results.xlsx
+++ b/Self_Learning_Testcases_and_results/Capstone_Self_Learning_Test_Cases_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jferg\Class12Capstone\Self_Learning_Testcases_and_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A227C44-EA18-44D6-893D-7FD74EA2F697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E83756B-D63E-48E9-9AD3-5EDFCCF4C180}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33720" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="58">
   <si>
     <t>Test Steps</t>
   </si>
@@ -1040,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7403B371-1F45-47AE-A3BA-31B379391E41}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1214,7 +1214,9 @@
         <v>42</v>
       </c>
       <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
+      <c r="E19" s="9" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="21" spans="1:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1349,7 +1351,9 @@
         <v>44</v>
       </c>
       <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
+      <c r="E32" s="9" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="33" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1503,7 +1507,9 @@
         <v>47</v>
       </c>
       <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
+      <c r="E48" s="9" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="9"/>

</xml_diff>